<commit_message>
Architecture Update version 2
</commit_message>
<xml_diff>
--- a/Zacher/Task Enumeration.xlsx
+++ b/Zacher/Task Enumeration.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zache_000\Documents\GitHub\Independent\Zacher\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="4260" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="152511" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -577,18 +582,18 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5">
+    <row r="1" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,7 +605,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:11" ht="16.5">
+    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -612,7 +617,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:11" ht="16.5">
+    <row r="3" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -622,7 +627,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="16.5">
+    <row r="4" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -657,7 +662,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -665,7 +670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -673,7 +678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -681,7 +686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -689,7 +694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -697,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>22</v>
       </c>
@@ -705,7 +710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>23</v>
       </c>
@@ -713,7 +718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>24</v>
       </c>
@@ -721,17 +726,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>26</v>
       </c>
@@ -746,7 +751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -754,52 +759,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Revert "Architecture Update version 2"
This reverts commit 028eae7b978ea9c4b873a6f19ab2796696ad4111.
</commit_message>
<xml_diff>
--- a/Zacher/Task Enumeration.xlsx
+++ b/Zacher/Task Enumeration.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zache_000\Documents\GitHub\Independent\Zacher\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
+    <workbookView xWindow="4260" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140000" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -582,18 +577,18 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="16.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +600,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="16.5">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -617,7 +612,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="16.5">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -627,7 +622,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="16.5">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -662,7 +657,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -670,7 +665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -678,7 +673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -686,7 +681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -694,7 +689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -702,7 +697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="B10" t="s">
         <v>22</v>
       </c>
@@ -710,7 +705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="B11" t="s">
         <v>23</v>
       </c>
@@ -718,7 +713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="B12" t="s">
         <v>24</v>
       </c>
@@ -726,17 +721,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="B13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="B15" t="s">
         <v>26</v>
       </c>
@@ -751,7 +746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -759,52 +754,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="B17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="B18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="B19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="C20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="C21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="C22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="C23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>17</v>
       </c>

</xml_diff>